<commit_message>
welcome back feature content
Former-commit-id: cc920fb04a31197d5e02998180c7f16ca829cc9b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_welcomeBackDefinitions.xlsx
+++ b/Docs/Content/HungryDragonContent_welcomeBackDefinitions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -173,9 +173,6 @@
     <t>CLUSTER_NON_PAYER</t>
   </si>
   <si>
-    <t>CLUSTER_GENERIC; CLUSTER_MINORS</t>
-  </si>
-  <si>
     <t>[enablePopup]</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>wb_non_payers_without_last_dragon</t>
+  </si>
+  <si>
+    <t>CLUSTER_GENERIC;CLUSTER_MINORS</t>
   </si>
 </sst>
 </file>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,25 +929,25 @@
         <v>42</v>
       </c>
       <c r="H11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="M11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="N11" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -1083,9 +1083,11 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="C16" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="8" t="b">
         <v>1</v>
@@ -1130,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>41</v>
@@ -1159,15 +1161,17 @@
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="C18" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="8" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
@@ -1198,7 +1202,7 @@
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1222,7 +1226,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>3</v>
@@ -1234,7 +1238,7 @@
         <v>4</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -1252,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" s="8" t="b">
         <v>1</v>
@@ -1276,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="8" t="b">
         <v>1</v>
@@ -1285,7 +1289,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="9">
@@ -1300,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="8" t="b">
         <v>1</v>
@@ -1324,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="8" t="b">
         <v>1</v>
@@ -1333,11 +1337,11 @@
         <v>4</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I28" s="9">
         <v>0</v>
@@ -1348,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="8" t="b">
         <v>1</v>
@@ -1372,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="8" t="b">
         <v>1</v>
@@ -1381,11 +1385,11 @@
         <v>6</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I30" s="9">
         <v>0</v>
@@ -1396,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="8" t="b">
         <v>1</v>
@@ -1408,7 +1412,7 @@
         <v>8</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H31" s="9">
         <v>1</v>
@@ -1509,7 +1513,7 @@
     <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1522,11 +1526,11 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F44" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G44" s="15"/>
       <c r="H44" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="2:11" ht="71.25" x14ac:dyDescent="0.25">
@@ -1537,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>3</v>
@@ -1566,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>13</v>
@@ -1588,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>13</v>
@@ -1597,7 +1601,7 @@
         <v>8</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G48" s="13">
         <v>1</v>
@@ -1611,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>13</v>
@@ -1632,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>13</v>
@@ -1641,7 +1645,7 @@
         <v>8</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G50" s="13">
         <v>1</v>

</xml_diff>